<commit_message>
Push before computer is wiped
</commit_message>
<xml_diff>
--- a/tables/shipping_assumptions_out.xlsx
+++ b/tables/shipping_assumptions_out.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\message_trade\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E53505A0-DDD1-4AE0-97A1-B1B9227BB1C1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75ADE41F-302F-40E5-9836-85EFDD8C079F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DA086400-0885-443B-9577-169FAEC3ED4A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="12795" xr2:uid="{DA086400-0885-443B-9577-169FAEC3ED4A}"/>
   </bookViews>
   <sheets>
     <sheet name="unformatted" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="59">
   <si>
     <t>Type of shipping</t>
   </si>
@@ -210,6 +210,18 @@
   </si>
   <si>
     <t>NCV</t>
+  </si>
+  <si>
+    <t>Liquid H2</t>
+  </si>
+  <si>
+    <t>Liquid hydrogen costs</t>
+  </si>
+  <si>
+    <t>Amos (1998)</t>
+  </si>
+  <si>
+    <t>https://www.energy.gov/sites/prod/files/2014/03/f12/25106.pdf</t>
   </si>
 </sst>
 </file>
@@ -447,34 +459,10 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -487,16 +475,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -511,6 +490,33 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -529,34 +535,40 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -874,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0421860-BB6E-4F63-A8C2-9665E0A1B8DD}">
-  <dimension ref="A2:M34"/>
+  <dimension ref="A2:M41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,17 +911,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32" t="s">
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -964,7 +976,7 @@
         <v>6894865.0396039598</v>
       </c>
       <c r="D4">
-        <f>C4*B31*B28</f>
+        <f>C4*B38*B35</f>
         <v>9.8464339777905845E-3</v>
       </c>
       <c r="E4">
@@ -992,11 +1004,11 @@
         <v>376219</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L12" si="0">$I$4*$J$4/$K$4</f>
+        <f t="shared" ref="L4:L15" si="0">$I$4*$J$4/$K$4</f>
         <v>1.342303286117926</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M12" si="1">$J$4*10^9/$K$4</f>
+        <f t="shared" ref="M4:M15" si="1">$J$4*10^9/$K$4</f>
         <v>13423.032861179259</v>
       </c>
     </row>
@@ -1012,7 +1024,7 @@
         <v>3678751.3306930694</v>
       </c>
       <c r="D5">
-        <f>C5*B32*B28</f>
+        <f>C5*B39*B35</f>
         <v>4.9033219791292555E-3</v>
       </c>
       <c r="E5">
@@ -1023,11 +1035,11 @@
         <v>96</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G12" si="2">F5*(0.1/(1-((1+0.1)^-25)))</f>
+        <f t="shared" ref="G5:G15" si="2">F5*(0.1/(1-((1+0.1)^-25)))</f>
         <v>10.576134930241999</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H12" si="3">G5/L5</f>
+        <f t="shared" ref="H5:H15" si="3">G5/L5</f>
         <v>7.8790948659816129</v>
       </c>
       <c r="I5" s="1">
@@ -1059,22 +1071,22 @@
         <v>35</v>
       </c>
       <c r="D6">
-        <f>0.1*10^9*B28</f>
+        <f>0.1*10^9*B35</f>
         <v>3.1735159817351598E-3</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>192000</v>
+        <v>960</v>
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
-        <v>21152.269860483997</v>
+        <v>105.76134930241999</v>
       </c>
       <c r="H6">
         <f t="shared" si="3"/>
-        <v>15758.189731963224</v>
+        <v>78.790948659816124</v>
       </c>
       <c r="I6" s="1">
         <v>100000</v>
@@ -1106,7 +1118,7 @@
         <v>7283748.837623762</v>
       </c>
       <c r="D7">
-        <f>C7*B31*B28</f>
+        <f>C7*B38*B35</f>
         <v>1.0401792004414755E-2</v>
       </c>
       <c r="E7">
@@ -1154,7 +1166,7 @@
         <v>3052216.3227722771</v>
       </c>
       <c r="D8">
-        <f>C8*B32*B28</f>
+        <f>C8*B39*B35</f>
         <v>4.0682280576129111E-3</v>
       </c>
       <c r="E8">
@@ -1201,22 +1213,22 @@
         <v>35</v>
       </c>
       <c r="D9">
-        <f>0.1*10^9*B28</f>
+        <f>0.1*10^9*B35</f>
         <v>3.1735159817351598E-3</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>1432000</v>
+        <v>716</v>
       </c>
       <c r="G9">
         <f t="shared" si="2"/>
-        <v>157760.67937610982</v>
+        <v>78.880339688054917</v>
       </c>
       <c r="H9">
         <f t="shared" si="3"/>
-        <v>117529.83175089239</v>
+        <v>58.764915875446199</v>
       </c>
       <c r="I9" s="1">
         <v>100000</v>
@@ -1248,7 +1260,7 @@
         <v>16810656.900990099</v>
       </c>
       <c r="D10">
-        <f>C10*B31*B28</f>
+        <f>C10*B38*B35</f>
         <v>2.4006999752441339E-2</v>
       </c>
       <c r="E10">
@@ -1296,7 +1308,7 @@
         <v>5594115.7841584161</v>
       </c>
       <c r="D11">
-        <f>C11*B32*B28</f>
+        <f>C11*B39*B35</f>
         <v>7.456266654775532E-3</v>
       </c>
       <c r="E11">
@@ -1343,22 +1355,22 @@
         <v>35</v>
       </c>
       <c r="D12">
-        <f>0.1*10^9*B28</f>
+        <f>0.1*10^9*B35</f>
         <v>3.1735159817351598E-3</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>4000000</v>
+        <v>2000</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>440672.28876008332</v>
+        <v>220.33614438004165</v>
       </c>
       <c r="H12">
         <f t="shared" si="3"/>
-        <v>328295.61941590055</v>
+        <v>164.14780970795027</v>
       </c>
       <c r="I12" s="1">
         <v>100000</v>
@@ -1378,55 +1390,173 @@
         <v>13423.032861179259</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <f>22565*1000/L13</f>
+        <v>16810656.900990099</v>
+      </c>
+      <c r="D13">
+        <f>C13*B41*B38</f>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f>C13*3.11*(10^-6)*(10^-3)</f>
+        <v>5.2281142962079204E-2</v>
+      </c>
+      <c r="F13">
+        <v>600</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>66.100843314012494</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>49.244342912385079</v>
+      </c>
+      <c r="I13" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J13">
+        <v>5.05</v>
+      </c>
+      <c r="K13">
+        <v>376219</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>1.342303286117926</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>13423.032861179259</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <f>7509*1000/L14</f>
+        <v>5594115.7841584161</v>
+      </c>
+      <c r="D14">
+        <f>C14*B42*B38</f>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f>2.575*C14*(10^-6)*(10^-3)</f>
+        <v>1.4404848144207921E-2</v>
+      </c>
+      <c r="F14">
+        <v>700</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>77.117650533014583</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="3"/>
+        <v>57.451733397782597</v>
+      </c>
+      <c r="I14" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J14">
+        <v>5.05</v>
+      </c>
+      <c r="K14">
+        <v>376219</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>1.342303286117926</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>13423.032861179259</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15">
+        <f>0.1*10^9*B38</f>
+        <v>4500000000</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>7000</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>771.1765053301458</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="3"/>
+        <v>574.51733397782596</v>
+      </c>
+      <c r="I15" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J15">
+        <v>5.05</v>
+      </c>
+      <c r="K15">
+        <v>376219</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>1.342303286117926</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>13423.032861179259</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="32"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
+      <c r="B19" s="30"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
         <v>19</v>
@@ -1434,71 +1564,106 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>39</v>
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>32</v>
       </c>
-      <c r="B28">
+      <c r="B35">
         <f>0.000000278/8760</f>
         <v>3.1735159817351596E-11</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>9</v>
       </c>
-      <c r="B31">
+      <c r="B38">
         <v>45</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>8</v>
       </c>
-      <c r="B32">
+      <c r="B39">
         <v>42</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C39" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
         <f>3.1*(10^-6) * 300000000000</f>
         <v>930000</v>
       </c>
@@ -1506,12 +1671,12 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="J2:M2"/>
-    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A19:B19"/>
     <mergeCell ref="G2:I2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B24" r:id="rId1" xr:uid="{B35DED55-B0CA-4F63-AE9F-5E05297D437A}"/>
-    <hyperlink ref="B25" r:id="rId2" display="C:\Users\shepard\Downloads\LNG_report_2015-01_web_tcm8-13833.pdf" xr:uid="{97F9267E-13DD-4333-928D-E79DDBE07A29}"/>
+    <hyperlink ref="B27" r:id="rId1" xr:uid="{B35DED55-B0CA-4F63-AE9F-5E05297D437A}"/>
+    <hyperlink ref="B28" r:id="rId2" display="C:\Users\shepard\Downloads\LNG_report_2015-01_web_tcm8-13833.pdf" xr:uid="{97F9267E-13DD-4333-928D-E79DDBE07A29}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1519,10 +1684,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8E7003-AC57-41E6-ABE0-D9706ADF5E6A}">
-  <dimension ref="A2:M23"/>
+  <dimension ref="A2:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,699 +1709,861 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="36" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="33" t="s">
+      <c r="D2" s="32"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="34"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="33" t="s">
+      <c r="G2" s="32"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="35"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="33"/>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="36"/>
+      <c r="B3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="40" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="str">
+      <c r="A4" s="45" t="str">
         <f>unformatted!A4</f>
         <v>Liquid</v>
       </c>
-      <c r="B4" s="20" t="str">
+      <c r="B4" s="12" t="str">
         <f>unformatted!B4</f>
         <v>Diesel</v>
       </c>
-      <c r="C4" s="39">
+      <c r="C4" s="21">
         <f>unformatted!C4</f>
         <v>6894865.0396039598</v>
       </c>
-      <c r="D4" s="40">
+      <c r="D4" s="22">
         <f>unformatted!D4</f>
         <v>9.8464339777905845E-3</v>
       </c>
-      <c r="E4" s="39">
+      <c r="E4" s="21">
         <f>unformatted!E4</f>
         <v>2.1443030273168316E-2</v>
       </c>
-      <c r="F4" s="40">
+      <c r="F4" s="22">
         <f>unformatted!F4</f>
         <v>76</v>
       </c>
-      <c r="G4" s="39">
+      <c r="G4" s="21">
         <f>unformatted!G4</f>
         <v>8.3727734864415826</v>
       </c>
-      <c r="H4" s="40">
+      <c r="H4" s="22">
         <f>unformatted!H4</f>
         <v>6.23761676890211</v>
       </c>
-      <c r="I4" s="24">
+      <c r="I4" s="13">
         <f>unformatted!I4</f>
         <v>100000</v>
       </c>
-      <c r="J4" s="21">
+      <c r="J4" s="12">
         <f>unformatted!J4</f>
         <v>5.05</v>
       </c>
-      <c r="K4" s="24">
+      <c r="K4" s="13">
         <f>unformatted!K4</f>
         <v>376219</v>
       </c>
-      <c r="L4" s="40">
+      <c r="L4" s="22">
         <f>unformatted!L4</f>
         <v>1.342303286117926</v>
       </c>
-      <c r="M4" s="45">
+      <c r="M4" s="27">
         <f>unformatted!M4</f>
         <v>13423.032861179259</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="str">
+      <c r="A5" s="46" t="str">
         <f>unformatted!A5</f>
         <v>Liquid</v>
       </c>
-      <c r="B5" s="22" t="str">
+      <c r="B5" s="8" t="str">
         <f>unformatted!B5</f>
         <v>LNG</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="23">
         <f>unformatted!C5</f>
         <v>3678751.3306930694</v>
       </c>
-      <c r="D5" s="42">
+      <c r="D5" s="24">
         <f>unformatted!D5</f>
         <v>4.9033219791292555E-3</v>
       </c>
-      <c r="E5" s="41">
+      <c r="E5" s="23">
         <f>unformatted!E5</f>
         <v>9.4727846765346544E-3</v>
       </c>
-      <c r="F5" s="42">
+      <c r="F5" s="24">
         <f>unformatted!F5</f>
         <v>96</v>
       </c>
-      <c r="G5" s="41">
+      <c r="G5" s="23">
         <f>unformatted!G5</f>
         <v>10.576134930241999</v>
       </c>
-      <c r="H5" s="42">
+      <c r="H5" s="24">
         <f>unformatted!H5</f>
         <v>7.8790948659816129</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="9">
         <f>unformatted!I5</f>
         <v>100000</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5" s="8">
         <f>unformatted!J5</f>
         <v>5.05</v>
       </c>
-      <c r="K5" s="17">
+      <c r="K5" s="9">
         <f>unformatted!K5</f>
         <v>376219</v>
       </c>
-      <c r="L5" s="42">
+      <c r="L5" s="24">
         <f>unformatted!L5</f>
         <v>1.342303286117926</v>
       </c>
-      <c r="M5" s="46">
+      <c r="M5" s="28">
         <f>unformatted!M5</f>
         <v>13423.032861179259</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="str">
+      <c r="A6" s="46" t="str">
         <f>unformatted!A6</f>
         <v>Liquid</v>
       </c>
-      <c r="B6" s="22" t="str">
+      <c r="B6" s="8" t="str">
         <f>unformatted!B6</f>
         <v>Electricity</v>
       </c>
-      <c r="C6" s="41" t="str">
+      <c r="C6" s="23" t="str">
         <f>unformatted!C6</f>
         <v>NA</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="24">
         <f>unformatted!D6</f>
         <v>3.1735159817351598E-3</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="23">
         <f>unformatted!E6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="42">
+      <c r="F6" s="24">
         <f>unformatted!F6</f>
-        <v>192000</v>
-      </c>
-      <c r="G6" s="41">
+        <v>960</v>
+      </c>
+      <c r="G6" s="23">
         <f>unformatted!G6</f>
-        <v>21152.269860483997</v>
-      </c>
-      <c r="H6" s="42">
+        <v>105.76134930241999</v>
+      </c>
+      <c r="H6" s="24">
         <f>unformatted!H6</f>
-        <v>15758.189731963224</v>
-      </c>
-      <c r="I6" s="17">
+        <v>78.790948659816124</v>
+      </c>
+      <c r="I6" s="9">
         <f>unformatted!I6</f>
         <v>100000</v>
       </c>
-      <c r="J6" s="16">
+      <c r="J6" s="8">
         <f>unformatted!J6</f>
         <v>5.05</v>
       </c>
-      <c r="K6" s="17">
+      <c r="K6" s="9">
         <f>unformatted!K6</f>
         <v>376219</v>
       </c>
-      <c r="L6" s="42">
+      <c r="L6" s="24">
         <f>unformatted!L6</f>
         <v>1.342303286117926</v>
       </c>
-      <c r="M6" s="46">
+      <c r="M6" s="28">
         <f>unformatted!M6</f>
         <v>13423.032861179259</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="str">
+      <c r="A7" s="46" t="str">
         <f>unformatted!A7</f>
         <v>Solid</v>
       </c>
-      <c r="B7" s="22" t="str">
+      <c r="B7" s="8" t="str">
         <f>unformatted!B7</f>
         <v>Diesel</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="23">
         <f>unformatted!C7</f>
         <v>7283748.837623762</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D7" s="24">
         <f>unformatted!D7</f>
         <v>1.0401792004414755E-2</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="23">
         <f>unformatted!E7</f>
         <v>2.2652458885009899E-2</v>
       </c>
-      <c r="F7" s="42">
+      <c r="F7" s="24">
         <f>unformatted!F7</f>
         <v>51.6</v>
       </c>
-      <c r="G7" s="41">
+      <c r="G7" s="23">
         <f>unformatted!G7</f>
         <v>5.6846725250050749</v>
       </c>
-      <c r="H7" s="42">
+      <c r="H7" s="24">
         <f>unformatted!H7</f>
         <v>4.2350134904651169</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="9">
         <f>unformatted!I7</f>
         <v>100000</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7" s="8">
         <f>unformatted!J7</f>
         <v>5.05</v>
       </c>
-      <c r="K7" s="17">
+      <c r="K7" s="9">
         <f>unformatted!K7</f>
         <v>376219</v>
       </c>
-      <c r="L7" s="42">
+      <c r="L7" s="24">
         <f>unformatted!L7</f>
         <v>1.342303286117926</v>
       </c>
-      <c r="M7" s="46">
+      <c r="M7" s="28">
         <f>unformatted!M7</f>
         <v>13423.032861179259</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="str">
+      <c r="A8" s="46" t="str">
         <f>unformatted!A8</f>
         <v>Solid</v>
       </c>
-      <c r="B8" s="22" t="str">
+      <c r="B8" s="8" t="str">
         <f>unformatted!B8</f>
         <v>LNG</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="23">
         <f>unformatted!C8</f>
         <v>3052216.3227722771</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="24">
         <f>unformatted!D8</f>
         <v>4.0682280576129111E-3</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="23">
         <f>unformatted!E8</f>
         <v>7.8594570311386128E-3</v>
       </c>
-      <c r="F8" s="42">
+      <c r="F8" s="24">
         <f>unformatted!F8</f>
         <v>71.599999999999994</v>
       </c>
-      <c r="G8" s="41">
+      <c r="G8" s="23">
         <f>unformatted!G8</f>
         <v>7.8880339688054901</v>
       </c>
-      <c r="H8" s="42">
+      <c r="H8" s="24">
         <f>unformatted!H8</f>
         <v>5.8764915875446189</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="9">
         <f>unformatted!I8</f>
         <v>100000</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8" s="8">
         <f>unformatted!J8</f>
         <v>5.05</v>
       </c>
-      <c r="K8" s="17">
+      <c r="K8" s="9">
         <f>unformatted!K8</f>
         <v>376219</v>
       </c>
-      <c r="L8" s="42">
+      <c r="L8" s="24">
         <f>unformatted!L8</f>
         <v>1.342303286117926</v>
       </c>
-      <c r="M8" s="46">
+      <c r="M8" s="28">
         <f>unformatted!M8</f>
         <v>13423.032861179259</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="str">
+      <c r="A9" s="46" t="str">
         <f>unformatted!A9</f>
         <v>Solid</v>
       </c>
-      <c r="B9" s="22" t="str">
+      <c r="B9" s="8" t="str">
         <f>unformatted!B9</f>
         <v>Electricity</v>
       </c>
-      <c r="C9" s="41" t="str">
+      <c r="C9" s="23" t="str">
         <f>unformatted!C9</f>
         <v>NA</v>
       </c>
-      <c r="D9" s="42">
+      <c r="D9" s="24">
         <f>unformatted!D9</f>
         <v>3.1735159817351598E-3</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="23">
         <f>unformatted!E9</f>
         <v>0</v>
       </c>
-      <c r="F9" s="42">
+      <c r="F9" s="24">
         <f>unformatted!F9</f>
-        <v>1432000</v>
-      </c>
-      <c r="G9" s="41">
+        <v>716</v>
+      </c>
+      <c r="G9" s="23">
         <f>unformatted!G9</f>
-        <v>157760.67937610982</v>
-      </c>
-      <c r="H9" s="42">
+        <v>78.880339688054917</v>
+      </c>
+      <c r="H9" s="24">
         <f>unformatted!H9</f>
-        <v>117529.83175089239</v>
-      </c>
-      <c r="I9" s="17">
+        <v>58.764915875446199</v>
+      </c>
+      <c r="I9" s="9">
         <f>unformatted!I9</f>
         <v>100000</v>
       </c>
-      <c r="J9" s="16">
+      <c r="J9" s="8">
         <f>unformatted!J9</f>
         <v>5.05</v>
       </c>
-      <c r="K9" s="17">
+      <c r="K9" s="9">
         <f>unformatted!K9</f>
         <v>376219</v>
       </c>
-      <c r="L9" s="42">
+      <c r="L9" s="24">
         <f>unformatted!L9</f>
         <v>1.342303286117926</v>
       </c>
-      <c r="M9" s="46">
+      <c r="M9" s="28">
         <f>unformatted!M9</f>
         <v>13423.032861179259</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="str">
+      <c r="A10" s="46" t="str">
         <f>unformatted!A10</f>
         <v>LNG</v>
       </c>
-      <c r="B10" s="22" t="str">
+      <c r="B10" s="8" t="str">
         <f>unformatted!B10</f>
         <v>Diesel</v>
       </c>
-      <c r="C10" s="41">
+      <c r="C10" s="23">
         <f>unformatted!C10</f>
         <v>16810656.900990099</v>
       </c>
-      <c r="D10" s="42">
+      <c r="D10" s="24">
         <f>unformatted!D10</f>
         <v>2.4006999752441339E-2</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="23">
         <f>unformatted!E10</f>
         <v>5.2281142962079204E-2</v>
       </c>
-      <c r="F10" s="42">
+      <c r="F10" s="24">
         <f>unformatted!F10</f>
         <v>180</v>
       </c>
-      <c r="G10" s="41">
+      <c r="G10" s="23">
         <f>unformatted!G10</f>
         <v>19.830252994203747</v>
       </c>
-      <c r="H10" s="42">
+      <c r="H10" s="24">
         <f>unformatted!H10</f>
         <v>14.773302873715522</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10" s="9">
         <f>unformatted!I10</f>
         <v>100000</v>
       </c>
-      <c r="J10" s="16">
+      <c r="J10" s="8">
         <f>unformatted!J10</f>
         <v>5.05</v>
       </c>
-      <c r="K10" s="17">
+      <c r="K10" s="9">
         <f>unformatted!K10</f>
         <v>376219</v>
       </c>
-      <c r="L10" s="42">
+      <c r="L10" s="24">
         <f>unformatted!L10</f>
         <v>1.342303286117926</v>
       </c>
-      <c r="M10" s="46">
+      <c r="M10" s="28">
         <f>unformatted!M10</f>
         <v>13423.032861179259</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="str">
+      <c r="A11" s="46" t="str">
         <f>unformatted!A11</f>
         <v>LNG</v>
       </c>
-      <c r="B11" s="22" t="str">
+      <c r="B11" s="8" t="str">
         <f>unformatted!B11</f>
         <v>LNG</v>
       </c>
-      <c r="C11" s="41">
+      <c r="C11" s="23">
         <f>unformatted!C11</f>
         <v>5594115.7841584161</v>
       </c>
-      <c r="D11" s="42">
+      <c r="D11" s="24">
         <f>unformatted!D11</f>
         <v>7.456266654775532E-3</v>
       </c>
-      <c r="E11" s="41">
+      <c r="E11" s="23">
         <f>unformatted!E11</f>
         <v>1.4404848144207921E-2</v>
       </c>
-      <c r="F11" s="42">
+      <c r="F11" s="24">
         <f>unformatted!F11</f>
         <v>200</v>
       </c>
-      <c r="G11" s="41">
+      <c r="G11" s="23">
         <f>unformatted!G11</f>
         <v>22.033614438004165</v>
       </c>
-      <c r="H11" s="42">
+      <c r="H11" s="24">
         <f>unformatted!H11</f>
         <v>16.414780970795025</v>
       </c>
-      <c r="I11" s="17">
+      <c r="I11" s="9">
         <f>unformatted!I11</f>
         <v>100000</v>
       </c>
-      <c r="J11" s="16">
+      <c r="J11" s="8">
         <f>unformatted!J11</f>
         <v>5.05</v>
       </c>
-      <c r="K11" s="17">
+      <c r="K11" s="9">
         <f>unformatted!K11</f>
         <v>376219</v>
       </c>
-      <c r="L11" s="42">
+      <c r="L11" s="24">
         <f>unformatted!L11</f>
         <v>1.342303286117926</v>
       </c>
-      <c r="M11" s="46">
+      <c r="M11" s="28">
         <f>unformatted!M11</f>
         <v>13423.032861179259</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="str">
+      <c r="A12" s="46" t="str">
         <f>unformatted!A12</f>
         <v>LNG</v>
       </c>
-      <c r="B12" s="23" t="str">
+      <c r="B12" s="8" t="str">
         <f>unformatted!B12</f>
         <v>Electricity</v>
       </c>
-      <c r="C12" s="43" t="str">
+      <c r="C12" s="23" t="str">
         <f>unformatted!C12</f>
         <v>NA</v>
       </c>
-      <c r="D12" s="44">
+      <c r="D12" s="24">
         <f>unformatted!D12</f>
         <v>3.1735159817351598E-3</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E12" s="23">
         <f>unformatted!E12</f>
         <v>0</v>
       </c>
-      <c r="F12" s="44">
+      <c r="F12" s="24">
         <f>unformatted!F12</f>
-        <v>4000000</v>
-      </c>
-      <c r="G12" s="43">
+        <v>2000</v>
+      </c>
+      <c r="G12" s="23">
         <f>unformatted!G12</f>
-        <v>440672.28876008332</v>
-      </c>
-      <c r="H12" s="44">
+        <v>220.33614438004165</v>
+      </c>
+      <c r="H12" s="24">
         <f>unformatted!H12</f>
-        <v>328295.61941590055</v>
-      </c>
-      <c r="I12" s="19">
+        <v>164.14780970795027</v>
+      </c>
+      <c r="I12" s="9">
         <f>unformatted!I12</f>
         <v>100000</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="8">
         <f>unformatted!J12</f>
         <v>5.05</v>
       </c>
-      <c r="K12" s="19">
+      <c r="K12" s="9">
         <f>unformatted!K12</f>
         <v>376219</v>
       </c>
-      <c r="L12" s="44">
+      <c r="L12" s="24">
         <f>unformatted!L12</f>
         <v>1.342303286117926</v>
       </c>
-      <c r="M12" s="47">
+      <c r="M12" s="28">
         <f>unformatted!M12</f>
         <v>13423.032861179259</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="29" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="46" t="str">
+        <f>unformatted!A13</f>
+        <v>Liquid H2</v>
+      </c>
+      <c r="B13" s="8" t="str">
+        <f>unformatted!B13</f>
+        <v>Diesel</v>
+      </c>
+      <c r="C13" s="23">
+        <f>unformatted!C13</f>
+        <v>16810656.900990099</v>
+      </c>
+      <c r="D13" s="24">
+        <f>unformatted!D13</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="23">
+        <f>unformatted!E13</f>
+        <v>5.2281142962079204E-2</v>
+      </c>
+      <c r="F13" s="24">
+        <f>unformatted!F13</f>
+        <v>600</v>
+      </c>
+      <c r="G13" s="23">
+        <f>unformatted!G13</f>
+        <v>66.100843314012494</v>
+      </c>
+      <c r="H13" s="24">
+        <f>unformatted!H13</f>
+        <v>49.244342912385079</v>
+      </c>
+      <c r="I13" s="9">
+        <f>unformatted!I13</f>
+        <v>100000</v>
+      </c>
+      <c r="J13" s="8">
+        <f>unformatted!J13</f>
+        <v>5.05</v>
+      </c>
+      <c r="K13" s="9">
+        <f>unformatted!K13</f>
+        <v>376219</v>
+      </c>
+      <c r="L13" s="24">
+        <f>unformatted!L13</f>
+        <v>1.342303286117926</v>
+      </c>
+      <c r="M13" s="28">
+        <f>unformatted!M13</f>
+        <v>13423.032861179259</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="46" t="str">
+        <f>unformatted!A14</f>
+        <v>Liquid H2</v>
+      </c>
+      <c r="B14" s="8" t="str">
+        <f>unformatted!B14</f>
+        <v>LNG</v>
+      </c>
+      <c r="C14" s="23">
+        <f>unformatted!C14</f>
+        <v>5594115.7841584161</v>
+      </c>
+      <c r="D14" s="24">
+        <f>unformatted!D14</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="23">
+        <f>unformatted!E14</f>
+        <v>1.4404848144207921E-2</v>
+      </c>
+      <c r="F14" s="24">
+        <f>unformatted!F14</f>
+        <v>700</v>
+      </c>
+      <c r="G14" s="23">
+        <f>unformatted!G14</f>
+        <v>77.117650533014583</v>
+      </c>
+      <c r="H14" s="24">
+        <f>unformatted!H14</f>
+        <v>57.451733397782597</v>
+      </c>
+      <c r="I14" s="9">
+        <f>unformatted!I14</f>
+        <v>100000</v>
+      </c>
+      <c r="J14" s="8">
+        <f>unformatted!J14</f>
+        <v>5.05</v>
+      </c>
+      <c r="K14" s="9">
+        <f>unformatted!K14</f>
+        <v>376219</v>
+      </c>
+      <c r="L14" s="24">
+        <f>unformatted!L14</f>
+        <v>1.342303286117926</v>
+      </c>
+      <c r="M14" s="28">
+        <f>unformatted!M14</f>
+        <v>13423.032861179259</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="47" t="str">
+        <f>unformatted!A15</f>
+        <v>Liquid H2</v>
+      </c>
+      <c r="B15" s="10" t="str">
+        <f>unformatted!B15</f>
+        <v>Electricity</v>
+      </c>
+      <c r="C15" s="25" t="str">
+        <f>unformatted!C15</f>
+        <v>NA</v>
+      </c>
+      <c r="D15" s="26">
+        <f>unformatted!D15</f>
+        <v>4500000000</v>
+      </c>
+      <c r="E15" s="25">
+        <f>unformatted!E15</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="26">
+        <f>unformatted!F15</f>
+        <v>7000</v>
+      </c>
+      <c r="G15" s="25">
+        <f>unformatted!G15</f>
+        <v>771.1765053301458</v>
+      </c>
+      <c r="H15" s="26">
+        <f>unformatted!H15</f>
+        <v>574.51733397782596</v>
+      </c>
+      <c r="I15" s="11">
+        <f>unformatted!I15</f>
+        <v>100000</v>
+      </c>
+      <c r="J15" s="10">
+        <f>unformatted!J15</f>
+        <v>5.05</v>
+      </c>
+      <c r="K15" s="11">
+        <f>unformatted!K15</f>
+        <v>376219</v>
+      </c>
+      <c r="L15" s="26">
+        <f>unformatted!L15</f>
+        <v>1.342303286117926</v>
+      </c>
+      <c r="M15" s="29">
+        <f>unformatted!M15</f>
+        <v>13423.032861179259</v>
+      </c>
+    </row>
+    <row r="17" spans="6:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="I14" s="29" t="s">
+      <c r="I17" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F15" s="10" t="s">
+    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F18" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G18" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="30">
+      <c r="H18" s="19">
         <f>0.0007</f>
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="I15" s="30">
-        <f>(H4*M4*H15)/10^9</f>
+      <c r="I18" s="19">
+        <f>(H4*M4*H18)/10^9</f>
         <v>5.860941440509107E-8</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F16" s="10" t="s">
+    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F19" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G19" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="30">
-        <f t="shared" ref="H16:H17" si="0">0.0007</f>
+      <c r="H19" s="19">
+        <f t="shared" ref="H19:H20" si="0">0.0007</f>
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="I16" s="30">
-        <f t="shared" ref="I16:I23" si="1">(H5*M5*H16)/10^9</f>
+      <c r="I19" s="19">
+        <f>(H5*M5*H19)/10^9</f>
         <v>7.4032944511693987E-8</v>
       </c>
     </row>
-    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F17" s="10" t="s">
+    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="G20" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H17" s="30">
+      <c r="H20" s="19">
         <f t="shared" si="0"/>
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="I17" s="30">
+      <c r="I20" s="19">
+        <f>(H6*M6*H20)/10^9</f>
+        <v>7.4032944511693979E-7</v>
+      </c>
+    </row>
+    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="19">
+        <v>1.4E-3</v>
+      </c>
+      <c r="I21" s="19">
+        <f>(H7*M7*H21)/10^9</f>
+        <v>7.9585415350071032E-8</v>
+      </c>
+    </row>
+    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="19">
+        <v>1.4E-3</v>
+      </c>
+      <c r="I22" s="19">
+        <f>(H8*M8*H22)/10^9</f>
+        <v>1.1043247556327685E-7</v>
+      </c>
+    </row>
+    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="19">
+        <v>1.4E-3</v>
+      </c>
+      <c r="I23" s="19">
+        <f>(H9*M9*H23)/10^9</f>
+        <v>1.1043247556327686E-6</v>
+      </c>
+    </row>
+    <row r="24" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="19">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="I24" s="19">
+        <f t="shared" ref="I24:I26" si="1">(H13*M13*H24)/10^9</f>
+        <v>4.627059031980874E-7</v>
+      </c>
+    </row>
+    <row r="25" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="19">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="I25" s="19">
         <f t="shared" si="1"/>
-        <v>1.4806588902338796E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F18" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="30">
-        <v>1.4E-3</v>
-      </c>
-      <c r="I18" s="30">
+        <v>5.3982355373110209E-7</v>
+      </c>
+    </row>
+    <row r="26" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="20">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="I26" s="20">
         <f t="shared" si="1"/>
-        <v>7.9585415350071032E-8</v>
-      </c>
-    </row>
-    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F19" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" s="30">
-        <v>1.4E-3</v>
-      </c>
-      <c r="I19" s="30">
-        <f t="shared" si="1"/>
-        <v>1.1043247556327685E-7</v>
-      </c>
-    </row>
-    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F20" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="30">
-        <v>1.4E-3</v>
-      </c>
-      <c r="I20" s="30">
-        <f t="shared" si="1"/>
-        <v>2.2086495112655373E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F21" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="30">
-        <v>6.9999999999999999E-4</v>
-      </c>
-      <c r="I21" s="30">
-        <f t="shared" si="1"/>
-        <v>1.3881177095942622E-7</v>
-      </c>
-    </row>
-    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F22" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" s="30">
-        <v>6.9999999999999999E-4</v>
-      </c>
-      <c r="I22" s="30">
-        <f t="shared" si="1"/>
-        <v>1.5423530106602911E-7</v>
-      </c>
-    </row>
-    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F23" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="31">
-        <v>6.9999999999999999E-4</v>
-      </c>
-      <c r="I23" s="31">
-        <f t="shared" si="1"/>
-        <v>3.0847060213205829E-3</v>
+        <v>5.3982355373110202E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>